<commit_message>
Control de cambios y To Do List de la Planificación
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891914F1-67C4-7743-8088-587A791EA045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68B0E16-F2D4-9F47-8848-40564E2470AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
@@ -274,6 +274,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -313,6 +319,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -352,6 +364,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -391,6 +409,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1473,7 +1497,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1539,8 +1563,18 @@
       <c r="F5" s="3">
         <v>44966</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="4">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E6" s="1"/>
@@ -1575,8 +1609,18 @@
       <c r="F10" s="3">
         <v>44971</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F11" s="3">
@@ -2463,23 +2507,23 @@
       <c r="F139" s="8"/>
       <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="L139" s="6" t="s">
         <v>5</v>
@@ -2520,23 +2564,23 @@
       <c r="F142" s="6"/>
       <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>0</v>
+        <v>164.0625</v>
       </c>
       <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>0</v>
+        <v>93.75</v>
       </c>
       <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>0</v>
+        <v>93.75</v>
       </c>
       <c r="J142" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>93.75</v>
       </c>
       <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>0</v>
+        <v>445.3125</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Control de cambios, Gannt
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68B0E16-F2D4-9F47-8848-40564E2470AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91AC2C5-BC60-F34D-8CEC-19C3CA57A703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -280,6 +280,9 @@
                 <c:pt idx="5">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -324,6 +327,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,6 +376,9 @@
                 <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -414,6 +423,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,7 +1509,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1525,20 +1537,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
@@ -1626,8 +1638,18 @@
       <c r="F11" s="3">
         <v>44972</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="4">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F12" s="3">
@@ -2501,42 +2523,42 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E139" s="8" t="s">
+      <c r="E139" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="8"/>
-      <c r="G139" s="6">
+      <c r="F139" s="7"/>
+      <c r="G139" s="8">
         <f>SUM(G5,G5:G137)</f>
-        <v>10.5</v>
-      </c>
-      <c r="H139" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="H139" s="8">
         <f>SUM(H5,H6:H138)</f>
-        <v>6</v>
-      </c>
-      <c r="I139" s="6">
+        <v>9</v>
+      </c>
+      <c r="I139" s="8">
         <f>SUM(I5,I6:I138)</f>
-        <v>6</v>
-      </c>
-      <c r="J139" s="6">
+        <v>9</v>
+      </c>
+      <c r="J139" s="8">
         <f>SUM(J5,J6:J138)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>28.5</v>
-      </c>
-      <c r="L139" s="6" t="s">
+        <v>40.5</v>
+      </c>
+      <c r="L139" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="6"/>
-      <c r="H140" s="6"/>
-      <c r="I140" s="6"/>
-      <c r="J140" s="6"/>
-      <c r="L140" s="6"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8"/>
+      <c r="J140" s="8"/>
+      <c r="L140" s="8"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
@@ -2555,45 +2577,50 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="6"/>
+      <c r="L141" s="8"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E142" s="6" t="s">
+      <c r="E142" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6">
+      <c r="F142" s="8"/>
+      <c r="G142" s="8">
         <f>PRODUCT(G139,G141)</f>
-        <v>164.0625</v>
-      </c>
-      <c r="H142" s="6">
+        <v>210.9375</v>
+      </c>
+      <c r="H142" s="8">
         <f>PRODUCT(H139,H141)</f>
-        <v>93.75</v>
-      </c>
-      <c r="I142" s="6">
+        <v>140.625</v>
+      </c>
+      <c r="I142" s="8">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>93.75</v>
-      </c>
-      <c r="J142" s="6">
+        <v>140.625</v>
+      </c>
+      <c r="J142" s="8">
         <f t="shared" si="0"/>
-        <v>93.75</v>
-      </c>
-      <c r="L142" s="6">
+        <v>140.625</v>
+      </c>
+      <c r="L142" s="8">
         <f>SUM(G142:J143)</f>
-        <v>445.3125</v>
+        <v>632.8125</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="G143" s="6"/>
-      <c r="H143" s="6"/>
-      <c r="I143" s="6"/>
-      <c r="J143" s="6"/>
-      <c r="L143" s="6"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
+      <c r="I143" s="8"/>
+      <c r="J143" s="8"/>
+      <c r="L143" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -2603,11 +2630,6 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Control de cambios, Herramienta de etiquetado, YOLO version 3 y 4
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E003B820-C43E-C44C-A2F5-0F190BE7BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69C59A-3384-E540-AD8F-6C5041977C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -293,6 +293,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1530,7 +1533,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1558,20 +1561,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
@@ -1727,7 +1730,9 @@
       <c r="F17" s="3">
         <v>44978</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.2">
@@ -2560,42 +2565,42 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E139" s="7" t="s">
+      <c r="E139" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>21</v>
-      </c>
-      <c r="H139" s="8">
+        <v>22</v>
+      </c>
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
         <v>11</v>
       </c>
-      <c r="I139" s="8">
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
         <v>11</v>
       </c>
-      <c r="J139" s="8">
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
         <v>11</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>54</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
@@ -2614,50 +2619,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>328.125</v>
-      </c>
-      <c r="H142" s="8">
+        <v>343.75</v>
+      </c>
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
         <v>171.875</v>
       </c>
-      <c r="I142" s="8">
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
         <v>171.875</v>
       </c>
-      <c r="J142" s="8">
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
         <v>171.875</v>
       </c>
-      <c r="L142" s="8">
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>843.75</v>
+        <v>859.375</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -2667,6 +2667,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Control de cambios, Etiquetado de Imagenes, Convertir Video en Frames, Preparar imagenes para entrenar la red
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69C59A-3384-E540-AD8F-6C5041977C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E801B739-BE83-F146-A4BD-90C14EE7DD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -296,7 +296,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,6 +355,12 @@
                 <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -400,6 +412,12 @@
                 <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -449,6 +467,12 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1533,7 +1557,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1561,20 +1585,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
@@ -1726,114 +1750,134 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F17" s="3">
         <v>44978</v>
       </c>
       <c r="G17" s="4">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F18" s="3">
         <v>44979</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F19" s="3">
         <v>44980</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F20" s="3">
         <v>44981</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F21" s="3">
         <v>44982</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4">
+        <v>2</v>
+      </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F22" s="3">
         <v>44983</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F23" s="3">
         <v>44984</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F24" s="3">
         <v>44985</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F25" s="3">
         <v>44986</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F26" s="3">
         <v>44987</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F27" s="3">
         <v>44988</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F28" s="3">
         <v>44989</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F29" s="3">
         <v>44990</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F30" s="3">
         <v>44991</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F31" s="3">
         <v>44992</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F32" s="3">
         <v>44993</v>
       </c>
@@ -2565,42 +2609,42 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E139" s="8" t="s">
+      <c r="E139" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="8"/>
-      <c r="G139" s="6">
+      <c r="F139" s="7"/>
+      <c r="G139" s="8">
         <f>SUM(G5,G5:G137)</f>
-        <v>22</v>
-      </c>
-      <c r="H139" s="6">
+        <v>28</v>
+      </c>
+      <c r="H139" s="8">
         <f>SUM(H5,H6:H138)</f>
-        <v>11</v>
-      </c>
-      <c r="I139" s="6">
+        <v>15</v>
+      </c>
+      <c r="I139" s="8">
         <f>SUM(I5,I6:I138)</f>
-        <v>11</v>
-      </c>
-      <c r="J139" s="6">
+        <v>15</v>
+      </c>
+      <c r="J139" s="8">
         <f>SUM(J5,J6:J138)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>55</v>
-      </c>
-      <c r="L139" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L139" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="6"/>
-      <c r="H140" s="6"/>
-      <c r="I140" s="6"/>
-      <c r="J140" s="6"/>
-      <c r="L140" s="6"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8"/>
+      <c r="J140" s="8"/>
+      <c r="L140" s="8"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
@@ -2619,45 +2663,50 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="6"/>
+      <c r="L141" s="8"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E142" s="6" t="s">
+      <c r="E142" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6">
+      <c r="F142" s="8"/>
+      <c r="G142" s="8">
         <f>PRODUCT(G139,G141)</f>
-        <v>343.75</v>
-      </c>
-      <c r="H142" s="6">
+        <v>437.5</v>
+      </c>
+      <c r="H142" s="8">
         <f>PRODUCT(H139,H141)</f>
-        <v>171.875</v>
-      </c>
-      <c r="I142" s="6">
+        <v>234.375</v>
+      </c>
+      <c r="I142" s="8">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>171.875</v>
-      </c>
-      <c r="J142" s="6">
+        <v>234.375</v>
+      </c>
+      <c r="J142" s="8">
         <f t="shared" si="0"/>
-        <v>171.875</v>
-      </c>
-      <c r="L142" s="6">
+        <v>234.375</v>
+      </c>
+      <c r="L142" s="8">
         <f>SUM(G142:J143)</f>
-        <v>859.375</v>
+        <v>1140.625</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="G143" s="6"/>
-      <c r="H143" s="6"/>
-      <c r="I143" s="6"/>
-      <c r="J143" s="6"/>
-      <c r="L143" s="6"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
+      <c r="I143" s="8"/>
+      <c r="J143" s="8"/>
+      <c r="L143" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -2667,11 +2716,6 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Control de cambios Inés
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D522719-D1C9-E943-A696-5AAEAE764324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4381AADF-93B7-4544-A0F2-D73C55C4BA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -404,7 +404,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,9 +1642,9 @@
   <dimension ref="E1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1669,20 +1672,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
@@ -2082,7 +2085,7 @@
         <v>2</v>
       </c>
       <c r="H40" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I40">
         <v>2</v>
@@ -2105,7 +2108,9 @@
       <c r="G42" s="4">
         <v>2</v>
       </c>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F43" s="3">
@@ -2762,42 +2767,42 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E139" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="E139" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
         <v>49.25</v>
       </c>
-      <c r="H139" s="8">
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>30</v>
-      </c>
-      <c r="I139" s="8">
+        <v>32</v>
+      </c>
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
         <v>29</v>
       </c>
-      <c r="J139" s="8">
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
         <v>26</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>134.25</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>136.25</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
@@ -2816,50 +2821,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
         <v>769.53125</v>
       </c>
-      <c r="H142" s="8">
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>468.75</v>
-      </c>
-      <c r="I142" s="8">
+        <v>500</v>
+      </c>
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
         <v>453.125</v>
       </c>
-      <c r="J142" s="8">
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
         <v>406.25</v>
       </c>
-      <c r="L142" s="8">
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>2097.65625</v>
+        <v>2128.90625</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -2869,6 +2869,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Jueves dia grande, grabación coche, control de cambios
</commit_message>
<xml_diff>
--- a/estadisticoHorasEmpleadas.xlsx
+++ b/estadisticoHorasEmpleadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/2do Cuatrimestre/Taller de Proyectos II/TallerDeProyectos2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8118E199-7C85-0B4E-BDFC-F73C0D6A015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DED4055-C362-774C-B5F8-1147B93CDE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5340" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -352,6 +352,12 @@
                 <c:pt idx="75">
                   <c:v>3.25</c:v>
                 </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -460,6 +466,12 @@
                 <c:pt idx="75">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="76">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -559,6 +571,12 @@
                 <c:pt idx="75">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -660,6 +678,12 @@
                 </c:pt>
                 <c:pt idx="75">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1741,9 +1765,9 @@
   <dimension ref="E1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I76" sqref="I76"/>
+      <selection pane="bottomLeft" activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1771,20 +1795,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
@@ -2559,112 +2583,132 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F81" s="3">
         <v>45042</v>
       </c>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G81" s="4">
+        <v>2</v>
+      </c>
+      <c r="H81" s="4">
+        <v>4</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+      <c r="J81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F82" s="3">
         <v>45043</v>
       </c>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G82" s="4">
+        <v>4</v>
+      </c>
+      <c r="H82" s="4">
+        <v>4</v>
+      </c>
+      <c r="I82">
+        <v>4</v>
+      </c>
+      <c r="J82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F83" s="3">
         <v>45044</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F84" s="3">
         <v>45045</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F85" s="3">
         <v>45046</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F86" s="3">
         <v>45047</v>
       </c>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F87" s="3">
         <v>45048</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F88" s="3">
         <v>45049</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F89" s="3">
         <v>45050</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F90" s="3">
         <v>45051</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F91" s="3">
         <v>45052</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F92" s="3">
         <v>45053</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F93" s="3">
         <v>45054</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F94" s="3">
         <v>45055</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F95" s="3">
         <v>45056</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F96" s="3">
         <v>45057</v>
       </c>
@@ -2948,42 +2992,42 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E139" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="E139" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>64</v>
-      </c>
-      <c r="H139" s="8">
+        <v>70</v>
+      </c>
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>58</v>
-      </c>
-      <c r="I139" s="8">
+        <v>66</v>
+      </c>
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
-        <v>45.5</v>
-      </c>
-      <c r="J139" s="8">
+        <v>51.5</v>
+      </c>
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="K139">
         <f>G139+I139+H139+J139</f>
-        <v>212.5</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>238.5</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
@@ -3002,50 +3046,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>1000</v>
-      </c>
-      <c r="H142" s="8">
+        <v>1093.75</v>
+      </c>
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>906.25</v>
-      </c>
-      <c r="I142" s="8">
+        <v>1031.25</v>
+      </c>
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>710.9375</v>
-      </c>
-      <c r="J142" s="8">
+        <v>804.6875</v>
+      </c>
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
-        <v>703.125</v>
-      </c>
-      <c r="L142" s="8">
+        <v>796.875</v>
+      </c>
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>3320.3125</v>
+        <v>3726.5625</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -3055,6 +3094,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>